<commit_message>
First results, GPU impl and handin 1
</commit_message>
<xml_diff>
--- a/results/cpu_comparison.xlsx
+++ b/results/cpu_comparison.xlsx
@@ -1,34 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\cuda-fun\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\cuda-fun\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1BC29E9B-1945-4380-93D4-9A187A86C1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5750EE61-AA91-4F80-8FEB-1A2160CC712C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="threads_results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>batch_size</t>
   </si>
   <si>
     <t>thread_count</t>
-  </si>
-  <si>
-    <t>execution_time</t>
   </si>
   <si>
     <t>MiBs</t>
@@ -52,6 +62,9 @@
     <t>it seems.</t>
   </si>
   <si>
+    <t>(in MiB/s) more peformant for Tasks compared to threads.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -71,17 +84,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Tasks performed better in average, probably because of thread creation overhead. Also the best result is around</t>
+      <t>Tasks performed better in average, probably because</t>
     </r>
   </si>
   <si>
-    <t>(in MiB/s) more peformant for Tasks compared to threads.</t>
+    <t xml:space="preserve"> of thread creation overhead. Also the best result is around</t>
+  </si>
+  <si>
+    <t>execution_time (s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -576,7 +592,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1078,7 +1096,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>execution_time</c:v>
+                  <c:v>execution_time (s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1421,6 +1439,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1006721200"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1993,7 +2012,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>execution_time</c:v>
+                  <c:v>execution_time (s)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3533,208 +3552,218 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>28140</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>80529</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Gruppieren 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D806EBAF-CA5B-F42F-1456-7B585BE8EED6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BBCF479-6C6D-E48D-FF4F-63BA3BEF8E40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="0" y="12383426"/>
+          <a:ext cx="7151914" cy="3481389"/>
+          <a:chOff x="0" y="12383426"/>
+          <a:chExt cx="7151914" cy="3481389"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="2" name="Diagramm 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D806EBAF-CA5B-F42F-1456-7B585BE8EED6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="0" y="12383426"/>
+          <a:ext cx="7151914" cy="3481389"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="5" name="Gerade Verbindung mit Pfeil 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9288FD99-9119-B236-2314-09CA2633FF4F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="4025473" y="12904374"/>
+            <a:ext cx="19050" cy="1125071"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent5"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>29936</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>14968</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>128589</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>391886</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>114982</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Gruppieren 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3098D53D-BAF4-412B-8AAB-772E2B080FCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E02E184-7DFE-CA1A-7049-A94AB49FA931}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Gerade Verbindung mit Pfeil 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9288FD99-9119-B236-2314-09CA2633FF4F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9210675" y="533400"/>
-          <a:ext cx="28575" cy="1409700"/>
+          <a:off x="29936" y="16751754"/>
+          <a:ext cx="7151914" cy="3529014"/>
+          <a:chOff x="29936" y="16751754"/>
+          <a:chExt cx="7151914" cy="3529014"/>
         </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Gerade Verbindung mit Pfeil 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CCE2960-FF77-489C-98DD-C44F40A0E4DE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6238875" y="4619625"/>
-          <a:ext cx="28575" cy="1409700"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="3" name="Diagramm 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3098D53D-BAF4-412B-8AAB-772E2B080FCD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr>
+            <a:graphicFrameLocks/>
+          </xdr:cNvGraphicFramePr>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="29936" y="16751754"/>
+          <a:ext cx="7151914" cy="3529014"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Gerade Verbindung mit Pfeil 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CCE2960-FF77-489C-98DD-C44F40A0E4DE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2168098" y="17242651"/>
+            <a:ext cx="28575" cy="1362075"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent5"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:D21" totalsRowShown="0">
-  <autoFilter ref="A1:D21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:D21" totalsRowShown="0">
+  <autoFilter ref="A1:D21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="batch_size"/>
-    <tableColumn id="2" name="thread_count"/>
-    <tableColumn id="3" name="execution_time" dataDxfId="1"/>
-    <tableColumn id="4" name="MiBs" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="batch_size"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="thread_count"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="execution_time (s)" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MiBs" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A24:D50" totalsRowShown="0">
-  <autoFilter ref="A24:D50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle2" displayName="Tabelle2" ref="A24:D50" totalsRowShown="0">
+  <autoFilter ref="A24:D50" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="batch_size"/>
-    <tableColumn id="2" name="task_count"/>
-    <tableColumn id="3" name="execution_time" dataDxfId="3"/>
-    <tableColumn id="4" name="MiBs" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="batch_size"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="task_count"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="execution_time (s)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="MiBs" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4036,11 +4065,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4059,10 +4091,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4275,7 +4307,7 @@
         <v>111.834</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -4289,7 +4321,7 @@
         <v>119.545</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>8</v>
       </c>
@@ -4303,7 +4335,7 @@
         <v>120.14400000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8</v>
       </c>
@@ -4317,7 +4349,7 @@
         <v>119.941</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -4330,11 +4362,8 @@
       <c r="D20" s="2">
         <v>117.52500000000001</v>
       </c>
-      <c r="F20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
@@ -4347,25 +4376,22 @@
       <c r="D21" s="2">
         <v>111.663</v>
       </c>
-      <c r="F21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
         <v>2</v>
       </c>
-      <c r="D24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -4379,7 +4405,7 @@
         <v>11.678000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -4393,7 +4419,7 @@
         <v>44.471200000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -4407,7 +4433,7 @@
         <v>119.60599999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -4421,7 +4447,7 @@
         <v>121.602</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -4435,7 +4461,7 @@
         <v>122.89400000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -4449,7 +4475,7 @@
         <v>123.361</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>1</v>
       </c>
@@ -4463,7 +4489,7 @@
         <v>123.661</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -4477,7 +4503,7 @@
         <v>123.621</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -4491,7 +4517,7 @@
         <v>123.30200000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -4505,7 +4531,7 @@
         <v>123.31699999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -4519,7 +4545,7 @@
         <v>44.640900000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -4533,7 +4559,7 @@
         <v>118.904</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -4547,7 +4573,7 @@
         <v>118.667</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -4561,7 +4587,7 @@
         <v>122.21</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -4575,7 +4601,7 @@
         <v>123.1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -4589,7 +4615,7 @@
         <v>123.084</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -4603,7 +4629,7 @@
         <v>123.06</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -4617,7 +4643,7 @@
         <v>123.093</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -4630,11 +4656,8 @@
       <c r="D43" s="2">
         <v>122.991</v>
       </c>
-      <c r="F43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8</v>
       </c>
@@ -4647,11 +4670,8 @@
       <c r="D44" s="2">
         <v>121.8</v>
       </c>
-      <c r="F44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>8</v>
       </c>
@@ -4664,11 +4684,8 @@
       <c r="D45" s="2">
         <v>122.77200000000001</v>
       </c>
-      <c r="F45" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>8</v>
       </c>
@@ -4682,7 +4699,7 @@
         <v>123.336</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>8</v>
       </c>
@@ -4696,7 +4713,7 @@
         <v>42.578499999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>8</v>
       </c>
@@ -4744,17 +4761,225 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="5">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="5">
         <f>D31/D18-1</f>
         <v>2.9273205486749276E-2</v>
       </c>
-      <c r="B54" t="s">
-        <v>11</v>
-      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65"/>
+      <c r="D65"/>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66"/>
+      <c r="D66"/>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C67"/>
+      <c r="D67"/>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68"/>
+      <c r="D68"/>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69"/>
+      <c r="D69"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C70"/>
+      <c r="D70"/>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C71"/>
+      <c r="D71"/>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C72"/>
+      <c r="D72"/>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C73"/>
+      <c r="D73"/>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C74"/>
+      <c r="D74"/>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C75"/>
+      <c r="D75"/>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C76"/>
+      <c r="D76"/>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C77"/>
+      <c r="D77"/>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C78"/>
+      <c r="D78"/>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C79"/>
+      <c r="D79"/>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C80"/>
+      <c r="D80"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C81"/>
+      <c r="D81"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C82"/>
+      <c r="D82"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C83"/>
+      <c r="D83"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84"/>
+      <c r="D84"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85"/>
+      <c r="D85"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C86"/>
+      <c r="D86"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C87"/>
+      <c r="D87"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C88"/>
+      <c r="D88"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C89"/>
+      <c r="D89"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C90"/>
+      <c r="D90"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C91"/>
+      <c r="D91"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C92"/>
+      <c r="D92"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C93"/>
+      <c r="D93"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C94"/>
+      <c r="D94"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C95"/>
+      <c r="D95"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C96"/>
+      <c r="D96"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C97"/>
+      <c r="D97"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C98"/>
+      <c r="D98"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C99"/>
+      <c r="D99"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C100"/>
+      <c r="D100"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C101"/>
+      <c r="D101"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C102"/>
+      <c r="D102"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C103"/>
+      <c r="D103"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C104"/>
+      <c r="D104"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C105"/>
+      <c r="D105"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C106"/>
+      <c r="D106"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107"/>
+      <c r="D107"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108"/>
+      <c r="D108"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109"/>
+      <c r="D109"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C110"/>
+      <c r="D110"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C111"/>
+      <c r="D111"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="2">
     <tablePart r:id="rId3"/>

</xml_diff>